<commit_message>
try catch + logs
</commit_message>
<xml_diff>
--- a/ExportedData.xlsx
+++ b/ExportedData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\AN_3\SEM_1\RPA\RPA-Project\RPA-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihai\Documents\GitHub\RPA-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3B8940-FE67-4C02-96F1-51540009A035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4774F8EE-B447-47AE-821B-A81C07FC7504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="2685" windowWidth="28080" windowHeight="15885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Followers" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>alex.popescu01</t>
   </si>
@@ -62,22 +62,43 @@
     <t>__vnp__</t>
   </si>
   <si>
-    <t>tomholland2013</t>
-  </si>
-  <si>
     <t>chrishemsworth</t>
   </si>
   <si>
-    <t>robertdowneyjr</t>
-  </si>
-  <si>
     <t>avengers</t>
   </si>
   <si>
     <t>marvelstudios</t>
   </si>
   <si>
-    <t>spidermanmovie</t>
+    <t>abdevilliers_38</t>
+  </si>
+  <si>
+    <t>avengers_fan_club777</t>
+  </si>
+  <si>
+    <t>mr_handsome_854</t>
+  </si>
+  <si>
+    <t>drawings_forever__</t>
+  </si>
+  <si>
+    <t>_ihab_43_</t>
+  </si>
+  <si>
+    <t>cristiano</t>
+  </si>
+  <si>
+    <t>therock</t>
+  </si>
+  <si>
+    <t>leomessi</t>
+  </si>
+  <si>
+    <t>k._.k._.gamming</t>
+  </si>
+  <si>
+    <t>jivar63</t>
   </si>
 </sst>
 </file>
@@ -395,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,57 +429,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -491,72 +547,72 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -576,32 +632,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>